<commit_message>
renamed:    FA.PY -> G12/anexos/FA.PY 	renamed:    calcular_phi.py -> G12/anexos/calcular_phi.py 	renamed:    graficas laboratorio.py -> G12/anexos/graficas laboratorio.py 	renamed:    visualizar_senales.py -> G12/anexos/visualizar_senales.py 	modified:   Libro1.xlsx 	modified:   informe.aux 	modified:   informe.log 	modified:   informe.out 	modified:   informe.pdf 	modified:   informe.synctex.gz 	modified:   informe.tex 	new file:   informe.toc 	new file:   out/image.png 	new file:   out/vibracion Forzada.png
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lunit\OneDrive\Desktop\laboratorio dinamica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3727318D-AA63-4B40-8505-2BC8D0B0AB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E00B2D85-9F1D-4AC7-A13E-4DB115DB5302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{98E019A0-0015-46D0-910D-F672A459B5FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{98E019A0-0015-46D0-910D-F672A459B5FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Vibracion libre" sheetId="2" r:id="rId1"/>
+    <sheet name="Vibracion Forzada" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Caso</t>
   </si>
   <si>
-    <t>f [Hz]</t>
-  </si>
-  <si>
     <t>Pm [N]</t>
   </si>
   <si>
@@ -56,9 +54,6 @@
     <t>FA</t>
   </si>
   <si>
-    <t>r = ω/ω_n</t>
-  </si>
-  <si>
     <t>φ_teo [°]</t>
   </si>
   <si>
@@ -74,9 +69,6 @@
     <t>datos adicionales</t>
   </si>
   <si>
-    <t>w_f = 2*pi*f</t>
-  </si>
-  <si>
     <t>Datos mecanismo</t>
   </si>
   <si>
@@ -89,20 +81,6 @@
     <t>Rango mov</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">w_n = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>√(K/m)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">m_barra </t>
   </si>
   <si>
@@ -119,13 +97,87 @@
   </si>
   <si>
     <t>kg</t>
+  </si>
+  <si>
+    <t>P_m</t>
+  </si>
+  <si>
+    <t>M_h*r*w_f^2</t>
+  </si>
+  <si>
+    <t>M_h</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>C_c</t>
+  </si>
+  <si>
+    <t>2m*w_n</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>f _f[Hz]</t>
+  </si>
+  <si>
+    <t>Tn</t>
+  </si>
+  <si>
+    <t>f_n</t>
+  </si>
+  <si>
+    <t>w_n</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>TEORICO</t>
+  </si>
+  <si>
+    <t>θ[RAD]</t>
+  </si>
+  <si>
+    <t>θ[°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w_n </t>
+  </si>
+  <si>
+    <t>w_f</t>
+  </si>
+  <si>
+    <t>r = ω_f/ω_n</t>
+  </si>
+  <si>
+    <t>ζ</t>
+  </si>
+  <si>
+    <t>abierta</t>
+  </si>
+  <si>
+    <t>cerrada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +198,20 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -178,25 +244,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,6 +350,240 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>710712</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>397088</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>150288</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49C8B35B-AACD-120D-6589-0C5628882339}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6044712" y="1626577"/>
+          <a:ext cx="5020376" cy="619211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>494809</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>61633</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>283119</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>109344</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3C4E130-AB4C-C33F-AE08-7A8F1B9DC0E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2709372" y="1788039"/>
+          <a:ext cx="4755287" cy="619211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>198904</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600344</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28EA9811-6E7F-6D41-0559-1CB439849C80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5971054" y="2714625"/>
+          <a:ext cx="1925440" cy="666843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>372595</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>86285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>249079</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>708</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE16BB4E-C414-9B95-3F52-56B5C321E7BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3039595" y="2572310"/>
+          <a:ext cx="2219635" cy="1057423"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>241020</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC4473D-B29F-E536-AB76-CD96E7ED9BAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7439026" y="1743075"/>
+          <a:ext cx="1831694" cy="685799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,256 +902,832 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9C52F0-1FE4-4166-938A-373B60559995}">
-  <dimension ref="A1:O14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640683E6-9516-497A-A99F-47B6AB0DBCF1}">
+  <dimension ref="D4:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E12"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E5" s="7"/>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3">
+        <f>H6*2*PI()</f>
+        <v>32.0570678937734</v>
+      </c>
+      <c r="G6" s="3">
+        <f>196/1000</f>
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="H6" s="3">
+        <f>1/G6</f>
+        <v>5.1020408163265305</v>
+      </c>
+      <c r="I6" s="8">
+        <f>ATAN((500/350)/119)</f>
+        <v>1.2004225278875898E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <f>I6/(2*PI())*360</f>
+        <v>0.68779144480384258</v>
+      </c>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="3">
+        <v>39.67</v>
+      </c>
+      <c r="G7" s="3">
+        <f>2*PI()/F7</f>
+        <v>0.15838631981798806</v>
+      </c>
+      <c r="H7" s="3">
+        <f>1/G7</f>
+        <v>6.3136765924554883</v>
+      </c>
+      <c r="I7" s="8">
+        <f>ATAN(15/845)</f>
+        <v>1.7749615056497612E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <f>I7/(2*PI())*360</f>
+        <v>1.0169780307191734</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>((-27.903/239.782)*2*PI() - PI()/2)</f>
+        <v>-2.3019592982699528</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9C52F0-1FE4-4166-938A-373B60559995}">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="M1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="16"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="C3" s="9">
         <v>4.2</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="L3">
-        <f>2*C3*PI()</f>
+      <c r="D3" s="11">
+        <f t="shared" ref="D3:D8" si="0">2*C3*PI()</f>
         <v>26.389378290154262</v>
       </c>
-      <c r="M3">
-        <f>B11/B14</f>
-        <v>1428.5714285714284</v>
+      <c r="E3" s="11">
+        <f t="shared" ref="E3:E8" si="1">0.05616*0.045*D3^2</f>
+        <v>1.7599402769460741</v>
+      </c>
+      <c r="F3" s="11">
+        <f>236.7626/350/119*180/PI()</f>
+        <v>0.32570222632758949</v>
+      </c>
+      <c r="G3" s="11">
+        <f>15/119*180/PI()</f>
+        <v>7.2221570814809644</v>
+      </c>
+      <c r="H3" s="11">
+        <f>1/((1-(I3)^2)^2+(2*0.00275*I3)^2)^(1/2)</f>
+        <v>1.7895353401925622</v>
+      </c>
+      <c r="I3" s="11">
+        <f t="shared" ref="I3:I8" si="2">D3/M3</f>
+        <v>0.66423464698719481</v>
+      </c>
+      <c r="J3" s="2">
+        <f>ATAN(2*(0.00275)*(I3)/(1-(I3^2)))*180/PI()</f>
+        <v>0.37458485998798541</v>
+      </c>
+      <c r="K3" s="11">
+        <f>((-27/231.284)*2*PI() - PI()/2)*180/PI()</f>
+        <v>-132.02625343733246</v>
+      </c>
+      <c r="M3" s="9">
+        <v>39.728999999999999</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9">
         <v>4.3</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="L4">
-        <f t="shared" ref="L4:L8" si="0">2*C4*PI()</f>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
         <v>27.017696820872221</v>
       </c>
-      <c r="M4">
-        <f>M3</f>
-        <v>1428.5714285714284</v>
+      <c r="E4" s="11">
+        <f t="shared" si="1"/>
+        <v>1.8447446553703466</v>
+      </c>
+      <c r="F4" s="11">
+        <f>498.764/350/119*180/PI()</f>
+        <v>0.68612418182624235</v>
+      </c>
+      <c r="G4" s="11">
+        <f>15/119*180/PI()</f>
+        <v>7.2221570814809644</v>
+      </c>
+      <c r="H4" s="11">
+        <f>1/((1-(I4)^2)^2+(2*0.00275*I4)^2)^(1/2)</f>
+        <v>1.8603081933722316</v>
+      </c>
+      <c r="I4" s="11">
+        <f t="shared" si="2"/>
+        <v>0.68004975762974706</v>
+      </c>
+      <c r="J4" s="2">
+        <f>ATAN(2*(0.00275)*(I4)/(1-(I4^2)))*180/PI()</f>
+        <v>0.39867078871807737</v>
+      </c>
+      <c r="K4" s="11">
+        <f>((-110.096/231.284)*2*PI() - PI()/2)*180/PI()</f>
+        <v>-261.36749623839091</v>
+      </c>
+      <c r="M4" s="9">
+        <v>39.728999999999999</v>
+      </c>
+      <c r="N4" s="9">
+        <v>2.7499999999999998E-3</v>
+      </c>
+      <c r="O4" s="1">
+        <v>2.6129999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9">
         <v>4.45</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="L5">
+      <c r="D5" s="11">
         <f t="shared" si="0"/>
         <v>27.960174616949161</v>
       </c>
-      <c r="M5">
-        <f>M4</f>
-        <v>1428.5714285714284</v>
+      <c r="E5" s="11">
+        <f t="shared" si="1"/>
+        <v>1.9756925926431201</v>
+      </c>
+      <c r="F5" s="11">
+        <f>435.5449/350/119*180/PI()</f>
+        <v>0.59915689215960355</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" ref="G5:G8" si="3">15/119*180/PI()</f>
+        <v>7.2221570814809644</v>
+      </c>
+      <c r="H5" s="11">
+        <f>1/((1-(I5)^2)^2+(2*0.00275*I5)^2)^(1/2)</f>
+        <v>1.9812996278519079</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.7037724235935755</v>
+      </c>
+      <c r="J5" s="2">
+        <f>ATAN(2*(0.00275)*(I5)/(1-(I5^2)))*180/PI()</f>
+        <v>0.43941207054949749</v>
+      </c>
+      <c r="K5" s="11">
+        <f>((-67.185/224.13)*2*PI()-PI()/2)*180/PI()</f>
+        <v>-197.91326462320973</v>
+      </c>
+      <c r="M5" s="9">
+        <v>39.728999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9">
         <v>4.2</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="L6">
+      <c r="D6" s="11">
         <f t="shared" si="0"/>
         <v>26.389378290154262</v>
       </c>
-      <c r="M6">
-        <f>M5</f>
-        <v>1428.5714285714284</v>
+      <c r="E6" s="11">
+        <f t="shared" si="1"/>
+        <v>1.7599402769460741</v>
+      </c>
+      <c r="F6" s="11">
+        <f>276/350/119*180/PI()</f>
+        <v>0.37967911514071362</v>
+      </c>
+      <c r="G6" s="11">
+        <f t="shared" si="3"/>
+        <v>7.2221570814809644</v>
+      </c>
+      <c r="H6" s="11">
+        <f>1/((1-(I6)^2)^2+(2*O4*I6)^2)^(1/2)</f>
+        <v>1.7895390557467579</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" si="2"/>
+        <v>0.66423464698719481</v>
+      </c>
+      <c r="J6" s="2">
+        <f>ATAN(2*(O4)*(I6)/(1-(I6^2)))*180/PI()</f>
+        <v>0.3559242159911899</v>
+      </c>
+      <c r="K6" s="11">
+        <f>((-112.393/236.99)*2*PI() - PI()/2)*180/PI()</f>
+        <v>-260.73074813283262</v>
+      </c>
+      <c r="M6" s="9">
+        <v>39.728999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
         <v>4.3</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="L7">
+      <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>27.017696820872221</v>
       </c>
-      <c r="M7">
-        <f>M6</f>
-        <v>1428.5714285714284</v>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
+        <v>1.8447446553703466</v>
+      </c>
+      <c r="F7" s="11">
+        <f>268.7626/350/119*180/PI()</f>
+        <v>0.36972299330042591</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="3"/>
+        <v>7.2221570814809644</v>
+      </c>
+      <c r="H7" s="11">
+        <f>1/((1-(I7)^2)^2+(2*O4*I7)^2)^(1/2)</f>
+        <v>1.8603125685526714</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="2"/>
+        <v>0.68004975762974706</v>
+      </c>
+      <c r="J7" s="2">
+        <f>ATAN(2*(O4)*(I7)/(1-(I7^2)))*180/PI()</f>
+        <v>0.37881032882130466</v>
+      </c>
+      <c r="K7" s="11">
+        <f>((-91.423/232.653)*2*PI() - PI()/2)</f>
+        <v>-4.039828105187091</v>
+      </c>
+      <c r="M7" s="9">
+        <v>39.728999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
         <v>4.45</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="L8">
+      <c r="D8" s="11">
         <f t="shared" si="0"/>
         <v>27.960174616949161</v>
       </c>
-      <c r="M8">
-        <f>M7</f>
-        <v>1428.5714285714284</v>
+      <c r="E8" s="11">
+        <f t="shared" si="1"/>
+        <v>1.9756925926431201</v>
+      </c>
+      <c r="F8" s="11">
+        <f>196.7626/350/119*180/PI()</f>
+        <v>0.27067626761154412</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="3"/>
+        <v>7.2221570814809644</v>
+      </c>
+      <c r="H8" s="11">
+        <f>1/((1-(I8)^2)^2+(2*O4*I8)^2)^(1/2)</f>
+        <v>1.9813052886176898</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="2"/>
+        <v>0.7037724235935755</v>
+      </c>
+      <c r="J8" s="2">
+        <f>ATAN(2*(O4)*(I8)/(1-(I8^2)))*180/PI()</f>
+        <v>0.41752215539740956</v>
+      </c>
+      <c r="K8" s="11">
+        <f>((65/223.473)*2*PI() - PI()/2)</f>
+        <v>0.256749036477951</v>
+      </c>
+      <c r="M8" s="9">
+        <v>39.728999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4" t="s">
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>3000</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B16" s="1">
+        <v>5.6160000000000002E-2</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>2.1</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B17" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="L1:O1"/>
+  <mergeCells count="3">
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E8F3B70BEA3A434BAD9E84C3E9DAC580" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="043bb5c95023d6f375bb73b2560ab904">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd3c33fe-e93b-4e7a-81e0-06652996fea7" xmlns:ns4="ee7019a3-2625-450a-8c7e-d17a1a992f0f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0adb61c8ac3509bd5b62140ce0ef936" ns3:_="" ns4:_="">
+    <xsd:import namespace="dd3c33fe-e93b-4e7a-81e0-06652996fea7"/>
+    <xsd:import namespace="ee7019a3-2625-450a-8c7e-d17a1a992f0f"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dd3c33fe-e93b-4e7a-81e0-06652996fea7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="15" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="17" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ee7019a3-2625-450a-8c7e-d17a1a992f0f" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Hash de la sugerencia para compartir" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dd3c33fe-e93b-4e7a-81e0-06652996fea7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2181E56A-6E69-46D0-B1DE-4030D619D9E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E027D3FF-F4A9-4D30-9DA9-A614DD4437A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dd3c33fe-e93b-4e7a-81e0-06652996fea7"/>
+    <ds:schemaRef ds:uri="ee7019a3-2625-450a-8c7e-d17a1a992f0f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90029DAD-5181-4852-93E9-2F88E6142A82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee7019a3-2625-450a-8c7e-d17a1a992f0f"/>
+    <ds:schemaRef ds:uri="dd3c33fe-e93b-4e7a-81e0-06652996fea7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>